<commit_message>
Se agregan ejecutables de APP y de API (server) e instrucciones para la BD
</commit_message>
<xml_diff>
--- a/server/BD.xlsx
+++ b/server/BD.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="BD" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>imagen</t>
   </si>
@@ -144,14 +144,37 @@
   </si>
   <si>
     <t>../../assets/images/brocoli.png</t>
+  </si>
+  <si>
+    <t>BD: tiendaDB</t>
+  </si>
+  <si>
+    <t>Collección: items</t>
+  </si>
+  <si>
+    <t>BD: users</t>
+  </si>
+  <si>
+    <t>Collección: users</t>
+  </si>
+  <si>
+    <t>db.items.insert({mail: "next.user1@nextu.com.co", user: "usuario uno", fecNacimiento: "1980-01-01", pass: "123"})</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -179,8 +202,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,356 +485,377 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2">
-        <v>7000</v>
-      </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2" t="str">
-        <f>"db.items.insert({"&amp;$A$1&amp;": '"&amp;A2&amp;"', "&amp;$B$1&amp;": '"&amp;B2&amp;"',"&amp;$C$1&amp;": '"&amp;C2&amp;"',"&amp;$D$1&amp;": '"&amp;D2&amp;"'})"</f>
-        <v>db.items.insert({imagen: '../../assets/images/arandanos.jpg', nombre: 'Arandanos',precio: '7000',unidades: '5'})</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3">
-        <v>2100</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="E3" t="str">
-        <f t="shared" ref="E3:E19" si="0">"db.items.insert({"&amp;$A$1&amp;": '"&amp;A3&amp;"', "&amp;$B$1&amp;": '"&amp;B3&amp;"',"&amp;$C$1&amp;": '"&amp;C3&amp;"',"&amp;$D$1&amp;": '"&amp;D3&amp;"'})"</f>
-        <v>db.items.insert({imagen: '../../assets/images/brocoli.png', nombre: 'Brocoli',precio: '2100',unidades: '10'})</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4">
-        <v>3000</v>
-      </c>
-      <c r="D4">
-        <v>12</v>
-      </c>
-      <c r="E4" t="str">
-        <f t="shared" si="0"/>
-        <v>db.items.insert({imagen: '../../assets/images/calabaza.jpg', nombre: 'Calabaza',precio: '3000',unidades: '12'})</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5">
-        <v>4000</v>
-      </c>
-      <c r="D5">
-        <v>14</v>
-      </c>
-      <c r="E5" t="str">
-        <f t="shared" si="0"/>
-        <v>db.items.insert({imagen: '../../assets/images/canela.jpg', nombre: 'Canela',precio: '4000',unidades: '14'})</v>
+      <c r="A4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6">
-        <v>1000</v>
-      </c>
-      <c r="D6">
-        <v>17</v>
-      </c>
-      <c r="E6" t="str">
-        <f t="shared" si="0"/>
-        <v>db.items.insert({imagen: '../../assets/images/cebolla.jpg', nombre: 'Cebolla',precio: '1000',unidades: '17'})</v>
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C7">
-        <v>1500</v>
+        <v>7000</v>
       </c>
       <c r="D7">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="0"/>
-        <v>db.items.insert({imagen: '../../assets/images/fresa.jpg', nombre: 'Fresa',precio: '1500',unidades: '23'})</v>
+        <f>"db.items.insert({"&amp;$A$6&amp;": '"&amp;A7&amp;"', "&amp;$B$6&amp;": '"&amp;B7&amp;"',"&amp;$C$6&amp;": '"&amp;C7&amp;"',"&amp;$D$6&amp;": '"&amp;D7&amp;"'})"</f>
+        <v>db.items.insert({imagen: '../../assets/images/arandanos.jpg', nombre: 'Arandanos',precio: '7000',unidades: '5'})</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C8">
-        <v>3400</v>
+        <v>2100</v>
       </c>
       <c r="D8">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="0"/>
-        <v>db.items.insert({imagen: '../../assets/images/kiwi.jpg', nombre: 'Kiwi',precio: '3400',unidades: '45'})</v>
+        <f t="shared" ref="E8:E24" si="0">"db.items.insert({"&amp;$A$6&amp;": '"&amp;A8&amp;"', "&amp;$B$6&amp;": '"&amp;B8&amp;"',"&amp;$C$6&amp;": '"&amp;C8&amp;"',"&amp;$D$6&amp;": '"&amp;D8&amp;"'})"</f>
+        <v>db.items.insert({imagen: '../../assets/images/brocoli.png', nombre: 'Brocoli',precio: '2100',unidades: '10'})</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C9">
-        <v>2500</v>
+        <v>3000</v>
       </c>
       <c r="D9">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v>db.items.insert({imagen: '../../assets/images/limon.jpg', nombre: 'Limon',precio: '2500',unidades: '21'})</v>
+        <v>db.items.insert({imagen: '../../assets/images/calabaza.jpg', nombre: 'Calabaza',precio: '3000',unidades: '12'})</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C10">
-        <v>2600</v>
+        <v>4000</v>
       </c>
       <c r="D10">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v>db.items.insert({imagen: '../../assets/images/lychee.jpg', nombre: 'Lychee',precio: '2600',unidades: '12'})</v>
+        <v>db.items.insert({imagen: '../../assets/images/canela.jpg', nombre: 'Canela',precio: '4000',unidades: '14'})</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C11">
-        <v>2300</v>
+        <v>1000</v>
       </c>
       <c r="D11">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
-        <v>db.items.insert({imagen: '../../assets/images/maiz.jpg', nombre: 'Maiz',precio: '2300',unidades: '43'})</v>
+        <v>db.items.insert({imagen: '../../assets/images/cebolla.jpg', nombre: 'Cebolla',precio: '1000',unidades: '17'})</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C12">
-        <v>1300</v>
+        <v>1500</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
-        <v>db.items.insert({imagen: '../../assets/images/manzana.jpg', nombre: 'Manzana',precio: '1300',unidades: '4'})</v>
+        <v>db.items.insert({imagen: '../../assets/images/fresa.jpg', nombre: 'Fresa',precio: '1500',unidades: '23'})</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C13">
-        <v>1200</v>
+        <v>3400</v>
       </c>
       <c r="D13">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
-        <v>db.items.insert({imagen: '../../assets/images/naranja.jpg', nombre: 'Naranja',precio: '1200',unidades: '8'})</v>
+        <v>db.items.insert({imagen: '../../assets/images/kiwi.jpg', nombre: 'Kiwi',precio: '3400',unidades: '45'})</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C14">
-        <v>800</v>
+        <v>2500</v>
       </c>
       <c r="D14">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
-        <v>db.items.insert({imagen: '../../assets/images/papa.jpg', nombre: 'Papa',precio: '800',unidades: '8'})</v>
+        <v>db.items.insert({imagen: '../../assets/images/limon.jpg', nombre: 'Limon',precio: '2500',unidades: '21'})</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C15">
-        <v>1700</v>
+        <v>2600</v>
       </c>
       <c r="D15">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
-        <v>db.items.insert({imagen: '../../assets/images/pasta.jpg', nombre: 'Pasta',precio: '1700',unidades: '8'})</v>
+        <v>db.items.insert({imagen: '../../assets/images/lychee.jpg', nombre: 'Lychee',precio: '2600',unidades: '12'})</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C16">
-        <v>1800</v>
+        <v>2300</v>
       </c>
       <c r="D16">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
-        <v>db.items.insert({imagen: '../../assets/images/pimienta.jpg', nombre: 'Pimienta',precio: '1800',unidades: '23'})</v>
+        <v>db.items.insert({imagen: '../../assets/images/maiz.jpg', nombre: 'Maiz',precio: '2300',unidades: '43'})</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C17">
-        <v>1700</v>
+        <v>1300</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
-        <v>db.items.insert({imagen: '../../assets/images/repollo.jpg', nombre: 'Repollo',precio: '1700',unidades: '5'})</v>
+        <v>db.items.insert({imagen: '../../assets/images/manzana.jpg', nombre: 'Manzana',precio: '1300',unidades: '4'})</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C18">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
-        <v>db.items.insert({imagen: '../../assets/images/tomate.jpg', nombre: 'Tomate',precio: '1000',unidades: '3'})</v>
+        <v>db.items.insert({imagen: '../../assets/images/naranja.jpg', nombre: 'Naranja',precio: '1200',unidades: '8'})</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19">
+        <v>800</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>db.items.insert({imagen: '../../assets/images/papa.jpg', nombre: 'Papa',precio: '800',unidades: '8'})</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20">
+        <v>1700</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>db.items.insert({imagen: '../../assets/images/pasta.jpg', nombre: 'Pasta',precio: '1700',unidades: '8'})</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21">
+        <v>1800</v>
+      </c>
+      <c r="D21">
+        <v>23</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>db.items.insert({imagen: '../../assets/images/pimienta.jpg', nombre: 'Pimienta',precio: '1800',unidades: '23'})</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22">
+        <v>1700</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>db.items.insert({imagen: '../../assets/images/repollo.jpg', nombre: 'Repollo',precio: '1700',unidades: '5'})</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23">
+        <v>1000</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="0"/>
+        <v>db.items.insert({imagen: '../../assets/images/tomate.jpg', nombre: 'Tomate',precio: '1000',unidades: '3'})</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>20</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B24" t="s">
         <v>38</v>
       </c>
-      <c r="C19">
+      <c r="C24">
         <v>1600</v>
       </c>
-      <c r="D19">
+      <c r="D24">
         <v>4</v>
       </c>
-      <c r="E19" t="str">
+      <c r="E24" t="str">
         <f t="shared" si="0"/>
         <v>db.items.insert({imagen: '../../assets/images/zanahoria.jpg', nombre: 'Zanahoria',precio: '1600',unidades: '4'})</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>